<commit_message>
Made some necessary changes in steps.java
</commit_message>
<xml_diff>
--- a/BikesOutput.xlsx
+++ b/BikesOutput.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="25">
   <si>
     <t>Royal Enfield Bullet 650</t>
   </si>
@@ -56,6 +56,45 @@
   </si>
   <si>
     <t>Rs. 2.30 Lakh</t>
+  </si>
+  <si>
+    <t>Expected Launch : Feb 2026</t>
+  </si>
+  <si>
+    <t>Expected Launch : Mar 2026</t>
+  </si>
+  <si>
+    <t>Expected Launch : Sep 2026</t>
+  </si>
+  <si>
+    <t>Expected Launch : Nov 2026</t>
+  </si>
+  <si>
+    <t>Expected Launch : Jan 2027</t>
+  </si>
+  <si>
+    <t>Feb 2026</t>
+  </si>
+  <si>
+    <t>2026-02-16 11:06:05</t>
+  </si>
+  <si>
+    <t>Mar 2026</t>
+  </si>
+  <si>
+    <t>2026-02-16 11:06:07</t>
+  </si>
+  <si>
+    <t>Sep 2026</t>
+  </si>
+  <si>
+    <t>Nov 2026</t>
+  </si>
+  <si>
+    <t>Jan 2027</t>
+  </si>
+  <si>
+    <t>2026-02-16 11:06:08</t>
   </si>
 </sst>
 </file>
@@ -428,7 +467,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A2:B7"/>
+  <dimension ref="A2:D7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A2" sqref="A2:B21"/>
@@ -443,6 +482,12 @@
       <c r="B2" t="s" s="0">
         <v>1</v>
       </c>
+      <c r="C2" t="s" s="0">
+        <v>17</v>
+      </c>
+      <c r="D2" t="s" s="0">
+        <v>18</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
@@ -451,6 +496,12 @@
       <c r="B3" t="s" s="0">
         <v>3</v>
       </c>
+      <c r="C3" t="s" s="0">
+        <v>19</v>
+      </c>
+      <c r="D3" t="s" s="0">
+        <v>20</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="s" s="0">
@@ -459,6 +510,12 @@
       <c r="B4" t="s" s="0">
         <v>5</v>
       </c>
+      <c r="C4" t="s" s="0">
+        <v>21</v>
+      </c>
+      <c r="D4" t="s" s="0">
+        <v>20</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="s" s="0">
@@ -467,6 +524,12 @@
       <c r="B5" t="s" s="0">
         <v>7</v>
       </c>
+      <c r="C5" t="s" s="0">
+        <v>22</v>
+      </c>
+      <c r="D5" t="s" s="0">
+        <v>20</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6" t="s" s="0">
@@ -475,6 +538,12 @@
       <c r="B6" t="s" s="0">
         <v>9</v>
       </c>
+      <c r="C6" t="s" s="0">
+        <v>22</v>
+      </c>
+      <c r="D6" t="s" s="0">
+        <v>20</v>
+      </c>
     </row>
     <row r="7">
       <c r="A7" t="s" s="0">
@@ -482,6 +551,12 @@
       </c>
       <c r="B7" t="s" s="0">
         <v>11</v>
+      </c>
+      <c r="C7" t="s" s="0">
+        <v>23</v>
+      </c>
+      <c r="D7" t="s" s="0">
+        <v>24</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Multi-browser support, retry analyzer
</commit_message>
<xml_diff>
--- a/BikesOutput.xlsx
+++ b/BikesOutput.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="342" uniqueCount="53">
   <si>
     <t>Royal Enfield Bullet 650</t>
   </si>
@@ -95,6 +95,90 @@
   </si>
   <si>
     <t>2026-02-16 11:06:08</t>
+  </si>
+  <si>
+    <t>2026-02-16 12:06:57</t>
+  </si>
+  <si>
+    <t>2026-02-16 12:06:58</t>
+  </si>
+  <si>
+    <t>2026-02-16 12:06:59</t>
+  </si>
+  <si>
+    <t>2026-02-16 12:07:00</t>
+  </si>
+  <si>
+    <t>2026-02-16 12:09:32</t>
+  </si>
+  <si>
+    <t>2026-02-16 12:09:34</t>
+  </si>
+  <si>
+    <t>2026-02-16 12:09:35</t>
+  </si>
+  <si>
+    <t>2026-02-16 12:10:56</t>
+  </si>
+  <si>
+    <t>2026-02-16 12:10:57</t>
+  </si>
+  <si>
+    <t>2026-02-16 12:10:58</t>
+  </si>
+  <si>
+    <t>2026-02-16 12:10:59</t>
+  </si>
+  <si>
+    <t>2026-02-16 12:21:37</t>
+  </si>
+  <si>
+    <t>2026-02-16 12:21:38</t>
+  </si>
+  <si>
+    <t>2026-02-16 14:02:10</t>
+  </si>
+  <si>
+    <t>2026-02-16 14:02:11</t>
+  </si>
+  <si>
+    <t>2026-02-16 14:07:25</t>
+  </si>
+  <si>
+    <t>2026-02-16 14:07:26</t>
+  </si>
+  <si>
+    <t>2026-02-16 14:08:32</t>
+  </si>
+  <si>
+    <t>2026-02-16 14:08:33</t>
+  </si>
+  <si>
+    <t>2026-02-16 14:08:34</t>
+  </si>
+  <si>
+    <t>2026-02-16 14:11:38</t>
+  </si>
+  <si>
+    <t>2026-02-16 14:11:39</t>
+  </si>
+  <si>
+    <t>2026-02-16 14:11:40</t>
+  </si>
+  <si>
+    <t>2026-02-16 14:12:59</t>
+  </si>
+  <si>
+    <t>2026-02-16 14:13:00</t>
+  </si>
+  <si>
+    <t>2026-02-16 14:13:01</t>
+  </si>
+  <si>
+    <t>2026-02-16 14:14:26</t>
+  </si>
+  <si>
+    <t>2026-02-16 14:14:27</t>
   </si>
 </sst>
 </file>
@@ -486,7 +570,7 @@
         <v>17</v>
       </c>
       <c r="D2" t="s" s="0">
-        <v>18</v>
+        <v>51</v>
       </c>
     </row>
     <row r="3">
@@ -500,7 +584,7 @@
         <v>19</v>
       </c>
       <c r="D3" t="s" s="0">
-        <v>20</v>
+        <v>52</v>
       </c>
     </row>
     <row r="4">
@@ -514,7 +598,7 @@
         <v>21</v>
       </c>
       <c r="D4" t="s" s="0">
-        <v>20</v>
+        <v>52</v>
       </c>
     </row>
     <row r="5">
@@ -528,7 +612,7 @@
         <v>22</v>
       </c>
       <c r="D5" t="s" s="0">
-        <v>20</v>
+        <v>52</v>
       </c>
     </row>
     <row r="6">
@@ -542,7 +626,7 @@
         <v>22</v>
       </c>
       <c r="D6" t="s" s="0">
-        <v>20</v>
+        <v>52</v>
       </c>
     </row>
     <row r="7">
@@ -556,7 +640,7 @@
         <v>23</v>
       </c>
       <c r="D7" t="s" s="0">
-        <v>24</v>
+        <v>52</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Edge headless flag applied
</commit_message>
<xml_diff>
--- a/BikesOutput.xlsx
+++ b/BikesOutput.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29530"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29426"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent>
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\2461919\Downloads\Cognizant-New-Identify-Bikes-Project-main\ZigwheelsAutomation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{67AAD8C6-E25E-4928-9218-0A38C5577080}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2CE495A5-3329-41DB-B3E6-1DDC86C423B9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,16 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="507" uniqueCount="76">
-  <si>
-    <t>Name</t>
-  </si>
-  <si>
-    <t>Price</t>
-  </si>
-  <si>
-    <t>Expected Launch Date</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="602" uniqueCount="84">
   <si>
     <t>Royal Enfield Bullet 650</t>
   </si>
@@ -37,217 +28,250 @@
     <t>Rs. 3.40 Lakh</t>
   </si>
   <si>
+    <t>Royal Enfield Flying Flea C6</t>
+  </si>
+  <si>
+    <t>Rs. 2.00 Lakh</t>
+  </si>
+  <si>
+    <t>Royal Enfield 250</t>
+  </si>
+  <si>
+    <t>Rs. 1.30 Lakh</t>
+  </si>
+  <si>
+    <t>Royal Enfield Interceptor 750</t>
+  </si>
+  <si>
+    <t>Rs. 3.80 Lakh</t>
+  </si>
+  <si>
+    <t>Royal Enfield Continental GT 750</t>
+  </si>
+  <si>
+    <t>Rs. 3.90 Lakh</t>
+  </si>
+  <si>
+    <t>Royal Enfield Flying Flea S6</t>
+  </si>
+  <si>
+    <t>Rs. 2.30 Lakh</t>
+  </si>
+  <si>
+    <t>Expected Launch : Feb 2026</t>
+  </si>
+  <si>
+    <t>Expected Launch : Mar 2026</t>
+  </si>
+  <si>
+    <t>Expected Launch : Sep 2026</t>
+  </si>
+  <si>
+    <t>Expected Launch : Nov 2026</t>
+  </si>
+  <si>
+    <t>Expected Launch : Jan 2027</t>
+  </si>
+  <si>
     <t>Feb 2026</t>
   </si>
   <si>
-    <t>2026-02-17 10:15:14</t>
-  </si>
-  <si>
-    <t>Royal Enfield Flying Flea C6</t>
-  </si>
-  <si>
-    <t>Rs. 2.00 Lakh</t>
+    <t>2026-02-16 11:06:05</t>
   </si>
   <si>
     <t>Mar 2026</t>
   </si>
   <si>
-    <t>2026-02-17 10:15:15</t>
-  </si>
-  <si>
-    <t>Royal Enfield 250</t>
-  </si>
-  <si>
-    <t>Rs. 1.30 Lakh</t>
+    <t>2026-02-16 11:06:07</t>
   </si>
   <si>
     <t>Sep 2026</t>
   </si>
   <si>
-    <t>Royal Enfield Interceptor 750</t>
-  </si>
-  <si>
-    <t>Rs. 3.80 Lakh</t>
-  </si>
-  <si>
     <t>Nov 2026</t>
   </si>
   <si>
-    <t>Royal Enfield Continental GT 750</t>
-  </si>
-  <si>
-    <t>Rs. 3.90 Lakh</t>
-  </si>
-  <si>
-    <t>2026-02-17 10:15:16</t>
-  </si>
-  <si>
-    <t>Royal Enfield Flying Flea S6</t>
-  </si>
-  <si>
-    <t>Rs. 2.30 Lakh</t>
-  </si>
-  <si>
     <t>Jan 2027</t>
   </si>
   <si>
-    <t>2026-02-18 09:53:48</t>
-  </si>
-  <si>
-    <t>2026-02-18 09:53:50</t>
-  </si>
-  <si>
-    <t>2026-02-18 09:53:51</t>
-  </si>
-  <si>
-    <t>2026-02-19 16:26:31</t>
-  </si>
-  <si>
-    <t>2026-02-19 16:26:35</t>
-  </si>
-  <si>
-    <t>2026-02-19 16:26:36</t>
-  </si>
-  <si>
-    <t>2026-02-19 16:26:37</t>
-  </si>
-  <si>
-    <t>2026-02-19 16:45:41</t>
-  </si>
-  <si>
-    <t>2026-02-19 16:45:43</t>
-  </si>
-  <si>
-    <t>2026-02-19 16:45:44</t>
-  </si>
-  <si>
-    <t>2026-02-19 16:50:24</t>
-  </si>
-  <si>
-    <t>2026-02-19 16:50:26</t>
-  </si>
-  <si>
-    <t>2026-02-19 16:50:27</t>
-  </si>
-  <si>
-    <t>2026-02-19 16:56:18</t>
-  </si>
-  <si>
-    <t>2026-02-19 16:56:19</t>
-  </si>
-  <si>
-    <t>2026-02-19 16:56:20</t>
-  </si>
-  <si>
-    <t>2026-02-19 16:58:09</t>
-  </si>
-  <si>
-    <t>2026-02-19 16:58:10</t>
-  </si>
-  <si>
-    <t>2026-02-19 16:58:11</t>
-  </si>
-  <si>
-    <t>2026-02-19 17:02:14</t>
-  </si>
-  <si>
-    <t>2026-02-19 17:04:37</t>
-  </si>
-  <si>
-    <t>2026-02-19 17:04:38</t>
-  </si>
-  <si>
-    <t>2026-02-19 17:09:26</t>
-  </si>
-  <si>
-    <t>2026-02-19 17:09:27</t>
-  </si>
-  <si>
-    <t>2026-02-19 17:12:53</t>
-  </si>
-  <si>
-    <t>2026-02-19 17:12:54</t>
-  </si>
-  <si>
-    <t>2026-02-19 17:12:55</t>
-  </si>
-  <si>
-    <t>2026-02-19 17:59:29</t>
-  </si>
-  <si>
-    <t>2026-02-19 17:59:30</t>
-  </si>
-  <si>
-    <t>2026-02-19 17:59:31</t>
-  </si>
-  <si>
-    <t>2026-02-19 18:02:46</t>
-  </si>
-  <si>
-    <t>2026-02-19 18:02:47</t>
-  </si>
-  <si>
-    <t>2026-02-19 18:02:48</t>
-  </si>
-  <si>
-    <t>2026-02-19 18:09:57</t>
-  </si>
-  <si>
-    <t>2026-02-19 18:09:58</t>
-  </si>
-  <si>
-    <t>2026-02-19 18:09:59</t>
-  </si>
-  <si>
-    <t>2026-02-19 18:13:09</t>
-  </si>
-  <si>
-    <t>2026-02-19 18:13:10</t>
-  </si>
-  <si>
-    <t>2026-02-19 18:13:11</t>
-  </si>
-  <si>
-    <t>2026-02-19 18:15:45</t>
-  </si>
-  <si>
-    <t>2026-02-19 18:15:49</t>
-  </si>
-  <si>
-    <t>2026-02-19 18:15:50</t>
-  </si>
-  <si>
-    <t>2026-02-19 18:15:51</t>
-  </si>
-  <si>
-    <t>2026-02-19 18:15:52</t>
-  </si>
-  <si>
-    <t>2026-02-19 18:19:18</t>
-  </si>
-  <si>
-    <t>2026-02-19 18:19:22</t>
-  </si>
-  <si>
-    <t>2026-02-19 18:19:23</t>
-  </si>
-  <si>
-    <t>2026-02-19 18:19:24</t>
-  </si>
-  <si>
-    <t>2026-02-19 18:19:25</t>
-  </si>
-  <si>
-    <t>2026-02-19 18:21:26</t>
-  </si>
-  <si>
-    <t>2026-02-19 18:21:29</t>
-  </si>
-  <si>
-    <t>2026-02-19 18:21:30</t>
-  </si>
-  <si>
-    <t>2026-02-19 18:21:31</t>
+    <t>2026-02-16 11:06:08</t>
+  </si>
+  <si>
+    <t>2026-02-16 12:06:57</t>
+  </si>
+  <si>
+    <t>2026-02-16 12:06:58</t>
+  </si>
+  <si>
+    <t>2026-02-16 12:06:59</t>
+  </si>
+  <si>
+    <t>2026-02-16 12:07:00</t>
+  </si>
+  <si>
+    <t>2026-02-16 12:09:32</t>
+  </si>
+  <si>
+    <t>2026-02-16 12:09:34</t>
+  </si>
+  <si>
+    <t>2026-02-16 12:09:35</t>
+  </si>
+  <si>
+    <t>2026-02-16 12:10:56</t>
+  </si>
+  <si>
+    <t>2026-02-16 12:10:57</t>
+  </si>
+  <si>
+    <t>2026-02-16 12:10:58</t>
+  </si>
+  <si>
+    <t>2026-02-16 12:10:59</t>
+  </si>
+  <si>
+    <t>2026-02-16 12:21:37</t>
+  </si>
+  <si>
+    <t>2026-02-16 12:21:38</t>
+  </si>
+  <si>
+    <t>2026-02-16 14:02:10</t>
+  </si>
+  <si>
+    <t>2026-02-16 14:02:11</t>
+  </si>
+  <si>
+    <t>2026-02-16 14:07:25</t>
+  </si>
+  <si>
+    <t>2026-02-16 14:07:26</t>
+  </si>
+  <si>
+    <t>2026-02-16 14:08:32</t>
+  </si>
+  <si>
+    <t>2026-02-16 14:08:33</t>
+  </si>
+  <si>
+    <t>2026-02-16 14:08:34</t>
+  </si>
+  <si>
+    <t>2026-02-16 14:11:38</t>
+  </si>
+  <si>
+    <t>2026-02-16 14:11:39</t>
+  </si>
+  <si>
+    <t>2026-02-16 14:11:40</t>
+  </si>
+  <si>
+    <t>2026-02-16 14:12:59</t>
+  </si>
+  <si>
+    <t>2026-02-16 14:13:00</t>
+  </si>
+  <si>
+    <t>2026-02-16 14:13:01</t>
+  </si>
+  <si>
+    <t>2026-02-16 14:14:26</t>
+  </si>
+  <si>
+    <t>2026-02-16 14:14:27</t>
+  </si>
+  <si>
+    <t>2026-02-16 17:33:29</t>
+  </si>
+  <si>
+    <t>2026-02-16 17:33:30</t>
+  </si>
+  <si>
+    <t>2026-02-16 17:33:31</t>
+  </si>
+  <si>
+    <t>2026-02-18 18:32:18</t>
+  </si>
+  <si>
+    <t>2026-02-18 18:32:19</t>
+  </si>
+  <si>
+    <t>2026-02-19 15:17:57</t>
+  </si>
+  <si>
+    <t>2026-02-19 15:18:00</t>
+  </si>
+  <si>
+    <t>2026-02-19 15:18:01</t>
+  </si>
+  <si>
+    <t>2026-02-19 15:18:02</t>
+  </si>
+  <si>
+    <t>2026-02-19 17:53:30</t>
+  </si>
+  <si>
+    <t>2026-02-19 17:53:31</t>
+  </si>
+  <si>
+    <t>2026-02-19 17:53:32</t>
+  </si>
+  <si>
+    <t>2026-02-20 09:48:04</t>
+  </si>
+  <si>
+    <t>2026-02-20 09:48:05</t>
+  </si>
+  <si>
+    <t>2026-02-20 09:48:06</t>
+  </si>
+  <si>
+    <t>2026-02-20 09:48:07</t>
+  </si>
+  <si>
+    <t>Royal Enfield Continental GT 450</t>
+  </si>
+  <si>
+    <t>Rs. 2.75 Lakh</t>
+  </si>
+  <si>
+    <t>Unrevealed</t>
+  </si>
+  <si>
+    <t>Royal Enfield Constellation</t>
+  </si>
+  <si>
+    <t>Rs. 3.50 Lakh</t>
+  </si>
+  <si>
+    <t>2026-02-20 09:50:45</t>
+  </si>
+  <si>
+    <t>2026-02-20 09:50:46</t>
+  </si>
+  <si>
+    <t>2026-02-20 09:50:47</t>
+  </si>
+  <si>
+    <t>2026-02-20 09:50:48</t>
+  </si>
+  <si>
+    <t>2026-02-20 10:01:11</t>
+  </si>
+  <si>
+    <t>2026-02-20 10:01:12</t>
+  </si>
+  <si>
+    <t>2026-02-20 10:01:13</t>
+  </si>
+  <si>
+    <t>2026-02-20 10:17:27</t>
+  </si>
+  <si>
+    <t>2026-02-20 10:17:28</t>
+  </si>
+  <si>
+    <t>2026-02-20 10:17:29</t>
   </si>
 </sst>
 </file>
@@ -255,16 +279,8 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="0"/>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
-      <sz val="11"/>
-      <color indexed="8"/>
-      <name val="Aptos Narrow"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
       <sz val="11"/>
       <color indexed="8"/>
       <name val="Aptos Narrow"/>
@@ -292,9 +308,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -629,113 +644,124 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D7"/>
+  <dimension ref="A2:D9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+      <selection activeCell="A2" sqref="A2:B21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <cols>
-    <col min="1" max="1" customWidth="true" width="36.08984375"/>
-    <col min="2" max="2" customWidth="true" width="21.90625"/>
-    <col min="3" max="3" customWidth="true" width="23.1796875"/>
-    <col min="4" max="4" customWidth="true" width="19.7265625"/>
-  </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="C2" t="s" s="0">
-        <v>5</v>
+        <v>17</v>
       </c>
       <c r="D2" t="s" s="0">
-        <v>72</v>
+        <v>81</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="C3" t="s" s="0">
-        <v>9</v>
+        <v>19</v>
       </c>
       <c r="D3" t="s" s="0">
-        <v>73</v>
+        <v>82</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s" s="0">
-        <v>11</v>
+        <v>4</v>
       </c>
       <c r="B4" t="s" s="0">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="C4" t="s" s="0">
-        <v>13</v>
+        <v>21</v>
       </c>
       <c r="D4" t="s" s="0">
-        <v>73</v>
+        <v>82</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s" s="0">
-        <v>14</v>
+        <v>6</v>
       </c>
       <c r="B5" t="s" s="0">
-        <v>15</v>
+        <v>7</v>
       </c>
       <c r="C5" t="s" s="0">
-        <v>16</v>
+        <v>22</v>
       </c>
       <c r="D5" t="s" s="0">
-        <v>74</v>
+        <v>82</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s" s="0">
-        <v>17</v>
+        <v>8</v>
       </c>
       <c r="B6" t="s" s="0">
-        <v>18</v>
+        <v>9</v>
       </c>
       <c r="C6" t="s" s="0">
-        <v>16</v>
+        <v>22</v>
       </c>
       <c r="D6" t="s" s="0">
-        <v>74</v>
+        <v>82</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s" s="0">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="B7" t="s" s="0">
-        <v>21</v>
+        <v>11</v>
       </c>
       <c r="C7" t="s" s="0">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D7" t="s" s="0">
-        <v>75</v>
+        <v>82</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="s" s="0">
+        <v>69</v>
+      </c>
+      <c r="B8" t="s" s="0">
+        <v>70</v>
+      </c>
+      <c r="C8" t="s" s="0">
+        <v>71</v>
+      </c>
+      <c r="D8" t="s" s="0">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="s" s="0">
+        <v>72</v>
+      </c>
+      <c r="B9" t="s" s="0">
+        <v>73</v>
+      </c>
+      <c r="C9" t="s" s="0">
+        <v>71</v>
+      </c>
+      <c r="D9" t="s" s="0">
+        <v>83</v>
       </c>
     </row>
   </sheetData>

</xml_diff>